<commit_message>
Faculty form creation completed
</commit_message>
<xml_diff>
--- a/ExamUsers.xlsx
+++ b/ExamUsers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ExamSGP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB579754-B328-4F04-A6EC-108BDA676EB2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09C90DF5-EACA-47B0-9637-B53CA99E0B8F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{FE088CB5-2602-4700-BB34-C6E88D28D567}"/>
   </bookViews>
@@ -399,7 +399,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Faculty view exams completed
</commit_message>
<xml_diff>
--- a/ExamUsers.xlsx
+++ b/ExamUsers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ExamSGP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09C90DF5-EACA-47B0-9637-B53CA99E0B8F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8180ED0-8BDD-45AC-B6EC-4F19CD863B9E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{FE088CB5-2602-4700-BB34-C6E88D28D567}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>#</t>
   </si>
@@ -34,6 +34,9 @@
   </si>
   <si>
     <t>Email ID</t>
+  </si>
+  <si>
+    <t>17it051@charusat.edu.in</t>
   </si>
 </sst>
 </file>
@@ -399,7 +402,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -424,7 +427,12 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B3" s="1"/>
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" s="1"/>
@@ -438,6 +446,7 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{93EB6AD5-1C71-4C7F-A82C-93D569DA80AD}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{C3437EF7-A43D-422C-981C-16B53CAE7822}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>